<commit_message>
Completed list of PrintFlags.
git-svn-id: svn://136.177.114.72/svn_GW/phast3/trunk@10423 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/src/phast/PhastFortran/PrintFlags.xlsx
+++ b/src/phast/PhastFortran/PrintFlags.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="244">
   <si>
     <t>PRIHDF_INTERMEDIATE</t>
   </si>
@@ -526,6 +526,240 @@
   </si>
   <si>
     <t>timprslm</t>
+  </si>
+  <si>
+    <t>pribcf</t>
+  </si>
+  <si>
+    <t>pric</t>
+  </si>
+  <si>
+    <t>prikd</t>
+  </si>
+  <si>
+    <t>prigfb</t>
+  </si>
+  <si>
+    <t>prip</t>
+  </si>
+  <si>
+    <t>privel</t>
+  </si>
+  <si>
+    <t>priwel</t>
+  </si>
+  <si>
+    <t>primaphead</t>
+  </si>
+  <si>
+    <t>primapv</t>
+  </si>
+  <si>
+    <t>print_bc_flows</t>
+  </si>
+  <si>
+    <t>prbcf</t>
+  </si>
+  <si>
+    <t>timprbcf</t>
+  </si>
+  <si>
+    <t>ntprbcf</t>
+  </si>
+  <si>
+    <t>print_components</t>
+  </si>
+  <si>
+    <t>prc</t>
+  </si>
+  <si>
+    <t>timprc</t>
+  </si>
+  <si>
+    <t>ntprc</t>
+  </si>
+  <si>
+    <t>print_conductances</t>
+  </si>
+  <si>
+    <t>prkd</t>
+  </si>
+  <si>
+    <t>timprkd</t>
+  </si>
+  <si>
+    <t>ntprkd</t>
+  </si>
+  <si>
+    <t>print_global_flow_balance</t>
+  </si>
+  <si>
+    <t>prgfb</t>
+  </si>
+  <si>
+    <t>timprgfb</t>
+  </si>
+  <si>
+    <t>ntprgfb</t>
+  </si>
+  <si>
+    <t>print_force_chemistry</t>
+  </si>
+  <si>
+    <t>prf_chem_phrq</t>
+  </si>
+  <si>
+    <t>print_heads</t>
+  </si>
+  <si>
+    <t>prp</t>
+  </si>
+  <si>
+    <t>timprp</t>
+  </si>
+  <si>
+    <t>ntprp</t>
+  </si>
+  <si>
+    <t>print_restart_hst</t>
+  </si>
+  <si>
+    <t>prcpd</t>
+  </si>
+  <si>
+    <t>pricpd</t>
+  </si>
+  <si>
+    <t>timprcpd</t>
+  </si>
+  <si>
+    <t>ntprcpd</t>
+  </si>
+  <si>
+    <t>print_velocities</t>
+  </si>
+  <si>
+    <t>prvel</t>
+  </si>
+  <si>
+    <t>timprvel</t>
+  </si>
+  <si>
+    <t>ntprvel</t>
+  </si>
+  <si>
+    <t>print_wells</t>
+  </si>
+  <si>
+    <t>prwel</t>
+  </si>
+  <si>
+    <t>timprwel</t>
+  </si>
+  <si>
+    <t>ntprwel</t>
+  </si>
+  <si>
+    <t>print_xyz_components</t>
+  </si>
+  <si>
+    <t>prmapc</t>
+  </si>
+  <si>
+    <t>primapcomp</t>
+  </si>
+  <si>
+    <t>timprmapc</t>
+  </si>
+  <si>
+    <t>ntprmapcomp</t>
+  </si>
+  <si>
+    <t>print_xyz_heads</t>
+  </si>
+  <si>
+    <t>prmaph</t>
+  </si>
+  <si>
+    <t>timprmaph</t>
+  </si>
+  <si>
+    <t>ntprmaphead</t>
+  </si>
+  <si>
+    <t>print_xyz_velocities</t>
+  </si>
+  <si>
+    <t>vecmap/primapv</t>
+  </si>
+  <si>
+    <t>timprmapv</t>
+  </si>
+  <si>
+    <t>ntprmapv</t>
+  </si>
+  <si>
+    <t>print_xyz_wells</t>
+  </si>
+  <si>
+    <t>prtem</t>
+  </si>
+  <si>
+    <t>pri_well_timser</t>
+  </si>
+  <si>
+    <t>timprtem</t>
+  </si>
+  <si>
+    <t>ntprtem</t>
+  </si>
+  <si>
+    <t>print_zone_flows_tsv</t>
+  </si>
+  <si>
+    <t>przf_tsv</t>
+  </si>
+  <si>
+    <t>timprzf_tsv</t>
+  </si>
+  <si>
+    <t>ntprzf_tsv</t>
+  </si>
+  <si>
+    <t>print_zone_flows</t>
+  </si>
+  <si>
+    <t>przf</t>
+  </si>
+  <si>
+    <t>timprzf</t>
+  </si>
+  <si>
+    <t>ntprzf</t>
+  </si>
+  <si>
+    <t>print_zone_flows_xyzt</t>
+  </si>
+  <si>
+    <t>przf_xyzt</t>
+  </si>
+  <si>
+    <t>pri_zf_xyzt</t>
+  </si>
+  <si>
+    <t>timprzf_xyzt</t>
+  </si>
+  <si>
+    <t>ntprzf_xyzt</t>
+  </si>
+  <si>
+    <t>none/prtichead</t>
+  </si>
+  <si>
+    <t>none/print_end_of_period</t>
+  </si>
+  <si>
+    <t>none/prt_bc</t>
   </si>
 </sst>
 </file>
@@ -845,17 +1079,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="15.88671875" customWidth="1"/>
@@ -1215,6 +1450,9 @@
       <c r="D29" t="s">
         <v>24</v>
       </c>
+      <c r="E29" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
@@ -1226,6 +1464,21 @@
       <c r="D30" t="s">
         <v>22</v>
       </c>
+      <c r="E30" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" t="s">
+        <v>166</v>
+      </c>
+      <c r="H30" t="s">
+        <v>177</v>
+      </c>
+      <c r="J30" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -1237,6 +1490,21 @@
       <c r="D31" t="s">
         <v>22</v>
       </c>
+      <c r="E31" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" t="s">
+        <v>180</v>
+      </c>
+      <c r="G31" t="s">
+        <v>167</v>
+      </c>
+      <c r="H31" t="s">
+        <v>181</v>
+      </c>
+      <c r="J31" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
@@ -1248,6 +1516,21 @@
       <c r="D32" t="s">
         <v>22</v>
       </c>
+      <c r="E32" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" t="s">
+        <v>184</v>
+      </c>
+      <c r="G32" t="s">
+        <v>168</v>
+      </c>
+      <c r="H32" t="s">
+        <v>185</v>
+      </c>
+      <c r="J32" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
@@ -1259,6 +1542,9 @@
       <c r="D33" t="s">
         <v>30</v>
       </c>
+      <c r="E33" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
@@ -1270,6 +1556,21 @@
       <c r="D34" t="s">
         <v>22</v>
       </c>
+      <c r="E34" t="s">
+        <v>187</v>
+      </c>
+      <c r="F34" t="s">
+        <v>188</v>
+      </c>
+      <c r="G34" t="s">
+        <v>169</v>
+      </c>
+      <c r="H34" t="s">
+        <v>189</v>
+      </c>
+      <c r="J34" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
@@ -1281,6 +1582,21 @@
       <c r="D35" t="s">
         <v>22</v>
       </c>
+      <c r="E35" t="s">
+        <v>191</v>
+      </c>
+      <c r="F35" t="s">
+        <v>192</v>
+      </c>
+      <c r="G35" t="s">
+        <v>160</v>
+      </c>
+      <c r="H35" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
@@ -1402,6 +1718,21 @@
       <c r="D40" t="s">
         <v>22</v>
       </c>
+      <c r="E40" t="s">
+        <v>193</v>
+      </c>
+      <c r="F40" t="s">
+        <v>194</v>
+      </c>
+      <c r="G40" t="s">
+        <v>170</v>
+      </c>
+      <c r="H40" t="s">
+        <v>195</v>
+      </c>
+      <c r="J40" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
@@ -1413,6 +1744,21 @@
       <c r="D41" t="s">
         <v>30</v>
       </c>
+      <c r="E41" t="s">
+        <v>197</v>
+      </c>
+      <c r="F41" t="s">
+        <v>198</v>
+      </c>
+      <c r="G41" t="s">
+        <v>199</v>
+      </c>
+      <c r="H41" t="s">
+        <v>200</v>
+      </c>
+      <c r="J41" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
@@ -1450,6 +1796,21 @@
       <c r="D43" t="s">
         <v>22</v>
       </c>
+      <c r="E43" t="s">
+        <v>202</v>
+      </c>
+      <c r="F43" t="s">
+        <v>203</v>
+      </c>
+      <c r="G43" t="s">
+        <v>171</v>
+      </c>
+      <c r="H43" t="s">
+        <v>204</v>
+      </c>
+      <c r="J43" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
@@ -1461,6 +1822,21 @@
       <c r="D44" t="s">
         <v>22</v>
       </c>
+      <c r="E44" t="s">
+        <v>206</v>
+      </c>
+      <c r="F44" t="s">
+        <v>207</v>
+      </c>
+      <c r="G44" t="s">
+        <v>172</v>
+      </c>
+      <c r="H44" t="s">
+        <v>208</v>
+      </c>
+      <c r="J44" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
@@ -1498,6 +1874,21 @@
       <c r="D46" t="s">
         <v>27</v>
       </c>
+      <c r="E46" t="s">
+        <v>210</v>
+      </c>
+      <c r="F46" t="s">
+        <v>211</v>
+      </c>
+      <c r="G46" t="s">
+        <v>212</v>
+      </c>
+      <c r="H46" t="s">
+        <v>213</v>
+      </c>
+      <c r="J46" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
@@ -1509,6 +1900,21 @@
       <c r="D47" t="s">
         <v>27</v>
       </c>
+      <c r="E47" t="s">
+        <v>215</v>
+      </c>
+      <c r="F47" t="s">
+        <v>216</v>
+      </c>
+      <c r="G47" t="s">
+        <v>173</v>
+      </c>
+      <c r="H47" t="s">
+        <v>217</v>
+      </c>
+      <c r="J47" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
@@ -1520,8 +1926,23 @@
       <c r="D48" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>219</v>
+      </c>
+      <c r="F48" t="s">
+        <v>220</v>
+      </c>
+      <c r="G48" t="s">
+        <v>174</v>
+      </c>
+      <c r="H48" t="s">
+        <v>221</v>
+      </c>
+      <c r="J48" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>100</v>
       </c>
@@ -1531,8 +1952,23 @@
       <c r="D49" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>223</v>
+      </c>
+      <c r="F49" t="s">
+        <v>224</v>
+      </c>
+      <c r="G49" t="s">
+        <v>225</v>
+      </c>
+      <c r="H49" t="s">
+        <v>226</v>
+      </c>
+      <c r="J49" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>101</v>
       </c>
@@ -1542,8 +1978,23 @@
       <c r="D50" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>232</v>
+      </c>
+      <c r="F50" t="s">
+        <v>233</v>
+      </c>
+      <c r="G50" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" t="s">
+        <v>234</v>
+      </c>
+      <c r="J50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>102</v>
       </c>
@@ -1553,8 +2004,23 @@
       <c r="D51" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>236</v>
+      </c>
+      <c r="F51" t="s">
+        <v>237</v>
+      </c>
+      <c r="G51" t="s">
+        <v>238</v>
+      </c>
+      <c r="H51" t="s">
+        <v>239</v>
+      </c>
+      <c r="J51" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>103</v>
       </c>
@@ -1564,8 +2030,23 @@
       <c r="D52" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>228</v>
+      </c>
+      <c r="F52" t="s">
+        <v>229</v>
+      </c>
+      <c r="G52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52" t="s">
+        <v>230</v>
+      </c>
+      <c r="J52" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>7</v>
       </c>
@@ -1574,6 +2055,9 @@
       </c>
       <c r="D53" t="s">
         <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>